<commit_message>
End of the project
</commit_message>
<xml_diff>
--- a/src/projet/document/planning et journal.xlsx
+++ b/src/projet/document/planning et journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\module_151_SCHNEIDER-main\module_151_SCHNEIDER\src\projet\document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\151 - Schneider\projet\module-151-exeossss\src\projet\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3D3B6A-C59C-4088-B9D2-E01C47389632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E98CCD9-7D9B-4C54-A755-DBFE7656A651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>Tâches</t>
   </si>
@@ -317,6 +317,42 @@
   </si>
   <si>
     <t>Mon professeur est passé au cours de la matinée afin de vérifier mon code et voir si j'avais bien tout compris</t>
+  </si>
+  <si>
+    <t>J'ai commencé la matinée par remettre en place mon infrastructure</t>
+  </si>
+  <si>
+    <t>Mon professeur est passé au cours de la matinée pour discuter avec moi de ce qu'il me fallait faire durant la remédiation</t>
+  </si>
+  <si>
+    <t>J'ai repris mes documents et ait relu ma documentation afin de me remttre dedans</t>
+  </si>
+  <si>
+    <t>J'ai termincé la matinée en mettant en forme mon code ainsi que mon infrastructure</t>
+  </si>
+  <si>
+    <t>J'ai passer un bon moment de l'après midi à résoudres les problèmes que j'avais avec la réservation</t>
+  </si>
+  <si>
+    <t>J'ai continuer en affichant les joueurs sur l'interface</t>
+  </si>
+  <si>
+    <t>J'ai terminé la journée en hébergeant mon site et en commencant la résolution de quelques problèmes du à l'hébergement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencé la journée en résoluant mes problèmes du à l'hébergement </t>
+  </si>
+  <si>
+    <t>J'ai rencontré des problèmes d'accent et de majuscule qui m'ont pris un certain temps à résoudre à l'aide de mon professeur</t>
+  </si>
+  <si>
+    <t>J'ai effectuer une démonstration de mon application auprès de mon professeur</t>
+  </si>
+  <si>
+    <t>J'ai corriger mon rapport de projet et l'ai finalisé</t>
+  </si>
+  <si>
+    <t>J'ai mis à jour le journal de travail</t>
   </si>
 </sst>
 </file>
@@ -1907,10 +1943,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A37" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,7 +2364,7 @@
         <v>92</v>
       </c>
       <c r="C41" s="13">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
@@ -2339,7 +2375,7 @@
         <v>93</v>
       </c>
       <c r="C42" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
@@ -2353,108 +2389,165 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="13"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="13"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="13"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="13"/>
+    <row r="44" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="13"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="13"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="13"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="13"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="13"/>
+      <c r="A49" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
+        <v>45782</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="12">
+        <v>45783</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="12">
+        <v>45783</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="12">
+        <v>45783</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="13">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="13"/>
+      <c r="A54" s="12">
+        <v>45783</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
+      <c r="A55" s="12">
+        <v>45783</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="B56" s="9"/>
-      <c r="C56" s="13"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="13"/>
+      <c r="C56" s="13">
+        <f>SUM(C8:C55)</f>
+        <v>57.75</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="13"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="13">
-        <f>SUM(C8:C43)</f>
-        <v>44.75</v>
-      </c>
+      <c r="B58" s="14"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="15"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="16"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="14"/>
+      <c r="B61" s="15"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
+      <c r="B62" s="16"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="16"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="16"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2470,6 +2563,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <INOU_x00cf_ xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
+    <NON xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
+    <TaxCatchAll xmlns="924ebf79-8ca5-43a7-b11c-cae8c16b2b70" xsi:nil="true"/>
+    <toutvabien xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <a xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
+    <_x002d__x002e__x002d_ xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60">.-.</_x002d__x002e__x002d_>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041433D532D33284694B8292187168088" ma:contentTypeVersion="20" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a6a15b9106ef78c138a0ab33249408c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="924ebf79-8ca5-43a7-b11c-cae8c16b2b70" xmlns:ns3="fcabc8dd-3274-4261-b688-fb49e1a84a60" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f299860b08438f464b66cb389ee0528" ns2:_="" ns3:_="">
     <xsd:import namespace="924ebf79-8ca5-43a7-b11c-cae8c16b2b70"/>
@@ -2738,32 +2856,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92433B2D-0774-4141-A340-826B2CF0D0B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fcabc8dd-3274-4261-b688-fb49e1a84a60"/>
+    <ds:schemaRef ds:uri="924ebf79-8ca5-43a7-b11c-cae8c16b2b70"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <INOU_x00cf_ xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
-    <NON xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
-    <TaxCatchAll xmlns="924ebf79-8ca5-43a7-b11c-cae8c16b2b70" xsi:nil="true"/>
-    <toutvabien xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <a xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60" xsi:nil="true"/>
-    <_x002d__x002e__x002d_ xmlns="fcabc8dd-3274-4261-b688-fb49e1a84a60">.-.</_x002d__x002e__x002d_>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64DE997C-CC40-4C9E-895E-C18775B049B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5622E8-3DF4-4B1B-82B9-E7FCE9ABFC72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2780,23 +2892,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64DE997C-CC40-4C9E-895E-C18775B049B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92433B2D-0774-4141-A340-826B2CF0D0B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fcabc8dd-3274-4261-b688-fb49e1a84a60"/>
-    <ds:schemaRef ds:uri="924ebf79-8ca5-43a7-b11c-cae8c16b2b70"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>